<commit_message>
Included Hi in the second row
</commit_message>
<xml_diff>
--- a/Interview Details.xlsx
+++ b/Interview Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Call From </t>
   </si>
@@ -29,6 +29,9 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Hi</t>
+  </si>
 </sst>
 </file>
 
@@ -38,7 +41,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Gautami"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -359,13 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -382,6 +387,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -393,7 +403,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -405,7 +415,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>